<commit_message>
removed temp files, readme updated
</commit_message>
<xml_diff>
--- a/temp/semantic_matching_results.xlsx
+++ b/temp/semantic_matching_results.xlsx
@@ -453,136 +453,136 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  no  dnd light showing</t>
+          <t xml:space="preserve"> add fresh paint</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Light Dimmer Not Functioning</t>
+          <t>Desk for Repaint</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.5509999990463257</v>
+        <v>0.5055999755859375</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  gas burner</t>
+          <t xml:space="preserve"> air con grill is loose</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Air conditioner is faulty</t>
+          <t>Air con Grill Loose</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.4805000126361847</v>
+        <v>0.9781000018119812</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  darjeeling tebags</t>
+          <t>Heineken</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Tea bags</t>
+          <t>Sweetener Sachet</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.4634000062942505</v>
+        <v>0.3255999982357025</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>set up the bait rail</t>
+          <t xml:space="preserve">  gas burner</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Tape to seal box</t>
+          <t>Air conditioner is faulty</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.4758999943733215</v>
+        <v>0.4805000126361847</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">  fan body needs paint job</t>
+          <t xml:space="preserve">  hair dryer</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ceiling Painting</t>
+          <t>Hair dryer not working</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.4948999881744385</v>
+        <v>0.9121000170707703</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Heineken</t>
+          <t xml:space="preserve">Veuve Clicquot Brut NV  </t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sweetener Sachet</t>
+          <t>Loofah</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.3255999982357025</v>
+        <v>0.2937999963760376</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  no space bar counter</t>
+          <t xml:space="preserve">  fan body needs paint job</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Bar Counter High Chair Defective</t>
+          <t>Ceiling Painting</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.6266000270843506</v>
+        <v>0.4948999881744385</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Veuve Clicquot Brut NV  </t>
+          <t xml:space="preserve"> bed ceiling repaint</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Loofah</t>
+          <t>Bedroom Ceiling Light Flickering</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.2937999963760376</v>
+        <v>0.6807000041007996</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>peppermint tea</t>
+          <t xml:space="preserve">  fan vent in kitchen</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Chamomile tea</t>
+          <t>Exhaust Fan</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.6674000024795532</v>
+        <v>0.6567999720573425</v>
       </c>
     </row>
     <row r="11">
@@ -603,256 +603,256 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> air con grill is loose</t>
+          <t xml:space="preserve">  no  dnd light showing</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Air con Grill Loose</t>
+          <t>Light Dimmer Not Functioning</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.9781000018119812</v>
+        <v>0.5509999990463257</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> air band dirty</t>
+          <t>BT</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Air con Grill Dirty</t>
+          <t>Express laundry service</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.6209999918937683</v>
+        <v>0.2673999965190887</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> door glass strip is broken</t>
+          <t xml:space="preserve"> add grout to tile corner</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Glass Wall - Broken or Cracked</t>
+          <t>Entrance Wall Socket</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.7461000084877014</v>
+        <v>0.4327999949455261</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> bed ceiling repaint</t>
+          <t>peppermint tea</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Bedroom Ceiling Light Flickering</t>
+          <t>Chamomile tea</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.6807000041007996</v>
+        <v>0.6674000024795532</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">  pond vacuum</t>
+          <t>Writing Table Light Fused</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Pond Water Low Level</t>
+          <t>Writing Table Light Fused</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.6601999998092651</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> add fresh paint</t>
+          <t xml:space="preserve"> blu tooth liight</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Desk for Repaint</t>
+          <t>Dental kit</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.5055999755859375</v>
+        <v>0.5746999979019165</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> buff gel</t>
+          <t xml:space="preserve"> door glass strip is broken</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Bath gel</t>
+          <t>Glass Wall - Broken or Cracked</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.6707999706268311</v>
+        <v>0.7461000084877014</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">  hair dryer</t>
+          <t>set up the bait rail</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Hair dryer not working</t>
+          <t>Tape to seal box</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.9121000170707703</v>
+        <v>0.4758999943733215</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> add grout to tile corner</t>
+          <t xml:space="preserve">  pond vacuum</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Entrance Wall Socket</t>
+          <t>Pond Water Low Level</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.4327999949455261</v>
+        <v>0.6601999998092651</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>bathroom crumb polish</t>
+          <t xml:space="preserve">  my basin tap is loose</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Cleaning of Bathroom</t>
+          <t>Basin Tap Loose</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.6427000164985657</v>
+        <v>0.9185000061988831</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> blu tooth liight</t>
+          <t xml:space="preserve">  no space bar counter</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Dental kit</t>
+          <t>Bar Counter High Chair Defective</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.5746999979019165</v>
+        <v>0.6266000270843506</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t xml:space="preserve">  my bag rack is loose</t>
+          <t>bathroom crumb polish</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Trash Bag</t>
+          <t>Cleaning of Bathroom</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.5766000151634216</v>
+        <v>0.6427000164985657</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve">  main lobby cleaning</t>
+          <t xml:space="preserve">  my bag rack is loose</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2nd Floor Guest Lift Lobby to Clean</t>
+          <t>Trash Bag</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.6998999714851379</v>
+        <v>0.5766000151634216</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve">  fan vent in kitchen</t>
+          <t xml:space="preserve">  darjeeling tebags</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Exhaust Fan</t>
+          <t>Tea bags</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.6567999720573425</v>
+        <v>0.4634000062942505</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>BT</t>
+          <t xml:space="preserve"> air band dirty</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Express laundry service</t>
+          <t>Air con Grill Dirty</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.2673999965190887</v>
+        <v>0.6209999918937683</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Writing Table Light Fused</t>
+          <t xml:space="preserve"> buff gel</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Writing Table Light Fused</t>
+          <t>Bath gel</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>0.6707999706268311</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t xml:space="preserve">  my basin tap is loose</t>
+          <t xml:space="preserve">  main lobby cleaning</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Basin Tap Loose</t>
+          <t>2nd Floor Guest Lift Lobby to Clean</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.9185000061988831</v>
+        <v>0.6998999714851379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed temp, updated main
</commit_message>
<xml_diff>
--- a/temp/semantic_matching_results.xlsx
+++ b/temp/semantic_matching_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,391 +453,391 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  pond vacuum</t>
+          <t xml:space="preserve">  main lobby cleaning</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Pond Water Low Level</t>
+          <t>2nd Floor Guest Lift Lobby to Clean</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.6601999998092651</v>
+        <v>0.6998999714851379</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> add grout to tile corner</t>
+          <t xml:space="preserve"> air con grill is loose</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Entrance Wall Socket</t>
+          <t>Air con Grill Loose</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.4327999949455261</v>
+        <v>0.9781000018119812</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>(Do Not Use)</t>
+          <t>bathroom crumb polish</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Rubbish to Clear</t>
+          <t>Cleaning of Bathroom</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.2867999970912933</v>
+        <v>0.6427000164985657</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  darjeeling tebags</t>
+          <t xml:space="preserve">  fan vent in kitchen</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Tea bags</t>
+          <t>Exhaust Fan</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.4634000062942505</v>
+        <v>0.6567999720573425</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">  my bag rack is loose</t>
+          <t xml:space="preserve"> blu tooth liight</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Trash Bag</t>
+          <t>Dental kit</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.5766000151634216</v>
+        <v>0.5746999979019165</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">  fan vent in kitchen</t>
+          <t xml:space="preserve"> air band dirty</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Exhaust Fan</t>
+          <t>Air con Grill Dirty</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.6567999720573425</v>
+        <v>0.6209999918937683</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  no  dnd light showing</t>
+          <t xml:space="preserve">  darjeeling tebags</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Light Dimmer Not Functioning</t>
+          <t>Tea bags</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.5509999990463257</v>
+        <v>0.4634000062942505</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Heineken</t>
+          <t xml:space="preserve"> add grout to tile corner</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sweetener Sachet</t>
+          <t>Entrance Wall Socket</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.3255999982357025</v>
+        <v>0.4327999949455261</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Veuve Clicquot Brut NV  </t>
+          <t xml:space="preserve">  my basin tap is loose</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Loofah</t>
+          <t>Basin Tap Loose</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.2937999963760376</v>
+        <v>0.9185000061988831</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SODA aSH</t>
+          <t>BT</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ashtray</t>
+          <t>Express laundry service</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5335000157356262</v>
+        <v>0.2673999965190887</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> add fresh paint</t>
+          <t xml:space="preserve">  gas burner</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Desk for Repaint</t>
+          <t>Air conditioner is faulty</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.5055999755859375</v>
+        <v>0.4805000126361847</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> bed ceiling repaint</t>
+          <t xml:space="preserve"> AC duct border to repaint</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Bedroom Ceiling Light Flickering</t>
+          <t>Desk for Repaint</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.6807000041007996</v>
+        <v>0.5903000235557556</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> AC duct border to repaint</t>
+          <t xml:space="preserve">  fan body needs paint job</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Desk for Repaint</t>
+          <t>Ceiling Painting</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.5903000235557556</v>
+        <v>0.4948999881744385</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> an edge tray</t>
+          <t>Heineken</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Bed Side Table Pull-out Tray</t>
+          <t>Sweetener Sachet</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.5882999897003174</v>
+        <v>0.3255999982357025</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BT</t>
+          <t>Writing Table Light Fused</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Express laundry service</t>
+          <t>Writing Table Light Fused</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.2673999965190887</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">  main lobby cleaning</t>
+          <t xml:space="preserve"> add fresh paint</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2nd Floor Guest Lift Lobby to Clean</t>
+          <t>Desk for Repaint</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.6998999714851379</v>
+        <v>0.5055999755859375</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>clear glass strip</t>
+          <t xml:space="preserve">Veuve Clicquot Brut NV  </t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Glass strip</t>
+          <t>Loofah</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.9309999942779541</v>
+        <v>0.2937999963760376</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>bathroom crumb polish</t>
+          <t xml:space="preserve">  hair dryer</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Cleaning of Bathroom</t>
+          <t>Hair dryer not working</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.6427000164985657</v>
+        <v>0.9121000170707703</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Writing Table Light Fused</t>
+          <t xml:space="preserve">  pond vacuum</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Writing Table Light Fused</t>
+          <t>Pond Water Low Level</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>0.6601999998092651</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> buff gel</t>
+          <t>peppermint tea</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Bath gel</t>
+          <t>Chamomile tea</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.6707999706268311</v>
+        <v>0.6674000024795532</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve">  my basin tap is loose</t>
+          <t xml:space="preserve"> door glass strip is broken</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Basin Tap Loose</t>
+          <t>Glass Wall - Broken or Cracked</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.9185000061988831</v>
+        <v>0.7461000084877014</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> door glass strip is broken</t>
+          <t xml:space="preserve"> bed ceiling repaint</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Glass Wall - Broken or Cracked</t>
+          <t>Bedroom Ceiling Light Flickering</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.7461000084877014</v>
+        <v>0.6807000041007996</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> blu tooth liight</t>
+          <t xml:space="preserve"> buff gel</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Dental kit</t>
+          <t>Bath gel</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.5746999979019165</v>
+        <v>0.6707999706268311</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve">  hair dryer</t>
+          <t>set up the bait rail</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Hair dryer not working</t>
+          <t>Tape to seal box</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.9121000170707703</v>
+        <v>0.4758999943733215</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t xml:space="preserve">  gas burner</t>
+          <t xml:space="preserve">  no  dnd light showing</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Air conditioner is faulty</t>
+          <t>Light Dimmer Not Functioning</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.4805000126361847</v>
+        <v>0.5509999990463257</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve">  fan body needs paint job</t>
+          <t xml:space="preserve">  my bag rack is loose</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Ceiling Painting</t>
+          <t>Trash Bag</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.4948999881744385</v>
+        <v>0.5766000151634216</v>
       </c>
     </row>
     <row r="28">
@@ -853,21 +853,6 @@
       </c>
       <c r="C28" t="n">
         <v>0.6266000270843506</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> air band dirty</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Air con Grill Dirty</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>0.6209999918937683</v>
       </c>
     </row>
   </sheetData>

</xml_diff>